<commit_message>
New Modifications and corrections bugs
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\OneDrive\Documentos\GitHub Projects\tupperwareentregas.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92AA44AC-EBA8-4F05-AC94-008E251DEB45}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18447B0D-2674-41C5-A604-2FE6D13129C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="20730" windowHeight="11310" xr2:uid="{213F8CAD-E5D0-4178-B457-4E9940FFC1C9}"/>
   </bookViews>
@@ -210,12 +210,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -532,8 +533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B2C11B9-46B5-458A-B55D-2AF83731467C}">
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,7 +596,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
       <c r="B2" s="1">
@@ -677,7 +678,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="A4" s="5">
         <v>3</v>
       </c>
       <c r="B4" s="1">
@@ -759,7 +760,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+      <c r="A6" s="5">
         <v>5</v>
       </c>
       <c r="B6" s="1">
@@ -841,7 +842,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+      <c r="A8" s="5">
         <v>7</v>
       </c>
       <c r="B8" s="1">
@@ -923,7 +924,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+      <c r="A10" s="5">
         <v>9</v>
       </c>
       <c r="B10" s="1">
@@ -1005,7 +1006,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+      <c r="A12" s="5">
         <v>11</v>
       </c>
       <c r="B12" s="1">
@@ -1087,7 +1088,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+      <c r="A14" s="5">
         <v>13</v>
       </c>
       <c r="B14" s="1">
@@ -1169,7 +1170,7 @@
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
+      <c r="A16" s="5">
         <v>15</v>
       </c>
       <c r="B16" s="1">
@@ -1251,7 +1252,7 @@
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
+      <c r="A18" s="5">
         <v>17</v>
       </c>
       <c r="B18" s="1">
@@ -1333,7 +1334,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
+      <c r="A20" s="5">
         <v>19</v>
       </c>
       <c r="B20" s="1">
@@ -1415,7 +1416,7 @@
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
+      <c r="A22" s="5">
         <v>21</v>
       </c>
       <c r="B22" s="1">
@@ -1497,7 +1498,7 @@
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
+      <c r="A24" s="5">
         <v>23</v>
       </c>
       <c r="B24" s="1">

</xml_diff>

<commit_message>
Update Worksheet to row back functions
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\OneDrive\Documentos\GitHub Projects\tupperwareentregas.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EA41CAA-F804-4691-BBCD-177898E51AAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4E978AA-E5D3-4138-8213-E2FD948DE78E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="20730" windowHeight="11310" xr2:uid="{213F8CAD-E5D0-4178-B457-4E9940FFC1C9}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="41">
   <si>
     <t>Nome</t>
   </si>
@@ -48,6 +48,9 @@
     <t>Consultora1</t>
   </si>
   <si>
+    <t>Pendente</t>
+  </si>
+  <si>
     <t>Consultora2</t>
   </si>
   <si>
@@ -57,25 +60,103 @@
     <t>Consultora4</t>
   </si>
   <si>
+    <t>null</t>
+  </si>
+  <si>
     <t>NumeroSequencial</t>
   </si>
   <si>
     <t>CodigoConsultora</t>
   </si>
   <si>
+    <t>DataEntrega</t>
+  </si>
+  <si>
+    <t>HorarioEntrega</t>
+  </si>
+  <si>
+    <t>NomeRecebidor</t>
+  </si>
+  <si>
+    <t>DocumentoRecebidor</t>
+  </si>
+  <si>
+    <t>observacao</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
     <t>Consultora5</t>
   </si>
   <si>
+    <t>Consultora6</t>
+  </si>
+  <si>
+    <t>Consultora7</t>
+  </si>
+  <si>
+    <t>Consultora8</t>
+  </si>
+  <si>
+    <t>Consultora9</t>
+  </si>
+  <si>
+    <t>Consultora10</t>
+  </si>
+  <si>
+    <t>Consultora11</t>
+  </si>
+  <si>
+    <t>Consultora12</t>
+  </si>
+  <si>
+    <t>Consultora13</t>
+  </si>
+  <si>
+    <t>Consultora14</t>
+  </si>
+  <si>
+    <t>Consultora15</t>
+  </si>
+  <si>
+    <t>Consultora16</t>
+  </si>
+  <si>
+    <t>Consultora17</t>
+  </si>
+  <si>
+    <t>Consultora18</t>
+  </si>
+  <si>
+    <t>Consultora19</t>
+  </si>
+  <si>
+    <t>Consultora20</t>
+  </si>
+  <si>
+    <t>Consultora21</t>
+  </si>
+  <si>
+    <t>Consultora22</t>
+  </si>
+  <si>
+    <t>Consultora23</t>
+  </si>
+  <si>
+    <t>Consultora24</t>
+  </si>
+  <si>
+    <t>qtdeVolume</t>
+  </si>
+  <si>
+    <t>Previsao</t>
+  </si>
+  <si>
     <t>15/04/2021</t>
   </si>
   <si>
-    <t>Previsao de Entrega</t>
-  </si>
-  <si>
-    <t>Teste</t>
-  </si>
-  <si>
-    <t>Observacao</t>
+    <t>Separação</t>
   </si>
 </sst>
 </file>
@@ -132,9 +213,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
@@ -452,70 +534,112 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B2C11B9-46B5-458A-B55D-2AF83731467C}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+      <c r="L1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
       <c r="B2" s="1">
         <v>1234</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1">
-        <v>8</v>
-      </c>
-      <c r="E2" s="1">
-        <v>342021</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="1">
+        <v>8</v>
+      </c>
+      <c r="K2" s="1">
+        <v>342021</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -523,45 +647,81 @@
         <v>12345</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="1">
-        <v>8</v>
-      </c>
-      <c r="E3" s="1">
-        <v>342021</v>
+        <v>8</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+        <v>8</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="1">
+        <v>8</v>
+      </c>
+      <c r="K3" s="1">
+        <v>342021</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
         <v>3</v>
       </c>
       <c r="B4" s="1">
         <v>12346</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="1">
-        <v>8</v>
-      </c>
-      <c r="E4" s="1">
-        <v>342021</v>
+        <v>8</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="1">
+        <v>8</v>
+      </c>
+      <c r="K4" s="1">
+        <v>342021</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -569,42 +729,857 @@
         <v>12347</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="1">
-        <v>8</v>
-      </c>
-      <c r="E5" s="1">
-        <v>342021</v>
+        <v>8</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+        <v>8</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" s="1">
+        <v>8</v>
+      </c>
+      <c r="K5" s="1">
+        <v>342021</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
         <v>5</v>
       </c>
       <c r="B6" s="1">
         <v>17903</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J6" s="1">
+        <v>8</v>
+      </c>
+      <c r="K6" s="1">
+        <v>342021</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>21237</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J7" s="1">
+        <v>8</v>
+      </c>
+      <c r="K7" s="1">
+        <v>342021</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>24571</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" s="1">
+        <v>8</v>
+      </c>
+      <c r="K8" s="1">
+        <v>342021</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>27905</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J9" s="1">
+        <v>8</v>
+      </c>
+      <c r="K9" s="1">
+        <v>342021</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
         <v>9</v>
       </c>
-      <c r="D6" s="1">
-        <v>8</v>
-      </c>
-      <c r="E6" s="1">
-        <v>342021</v>
-      </c>
-      <c r="F6" s="1" t="s">
+      <c r="B10" s="1">
+        <v>31239</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J10" s="1">
+        <v>8</v>
+      </c>
+      <c r="K10" s="1">
+        <v>342021</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>34573</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J11" s="1">
+        <v>8</v>
+      </c>
+      <c r="K11" s="1">
+        <v>342021</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>37907</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J12" s="1">
+        <v>8</v>
+      </c>
+      <c r="K12" s="1">
+        <v>342021</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>10</v>
+      <c r="B13" s="1">
+        <v>41241</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J13" s="1">
+        <v>8</v>
+      </c>
+      <c r="K13" s="1">
+        <v>342021</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1">
+        <v>44575</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J14" s="1">
+        <v>8</v>
+      </c>
+      <c r="K14" s="1">
+        <v>342021</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
+        <v>47909</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J15" s="1">
+        <v>8</v>
+      </c>
+      <c r="K15" s="1">
+        <v>342021</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1">
+        <v>51243</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J16" s="1">
+        <v>8</v>
+      </c>
+      <c r="K16" s="1">
+        <v>342021</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1">
+        <v>54577</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J17" s="1">
+        <v>8</v>
+      </c>
+      <c r="K17" s="1">
+        <v>342021</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1">
+        <v>57911</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J18" s="1">
+        <v>8</v>
+      </c>
+      <c r="K18" s="1">
+        <v>342021</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1">
+        <v>61245</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J19" s="1">
+        <v>8</v>
+      </c>
+      <c r="K19" s="1">
+        <v>342021</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1">
+        <v>64579</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J20" s="1">
+        <v>8</v>
+      </c>
+      <c r="K20" s="1">
+        <v>342021</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1">
+        <v>67913</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J21" s="1">
+        <v>8</v>
+      </c>
+      <c r="K21" s="1">
+        <v>342021</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1">
+        <v>71247</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J22" s="1">
+        <v>8</v>
+      </c>
+      <c r="K22" s="1">
+        <v>342021</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1">
+        <v>74581</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J23" s="1">
+        <v>8</v>
+      </c>
+      <c r="K23" s="1">
+        <v>342021</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1">
+        <v>77915</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J24" s="1">
+        <v>8</v>
+      </c>
+      <c r="K24" s="1">
+        <v>342021</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1">
+        <v>81249</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J25" s="1">
+        <v>8</v>
+      </c>
+      <c r="K25" s="1">
+        <v>342021</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>